<commit_message>
Added in Guardian doc 1 new skills
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Guardian/Documentation/GuardianSkills.xlsx
+++ b/GameDesign/Class/Guardian/Documentation/GuardianSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1-ArmorStrengthening" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="3-Backfire" sheetId="3" r:id="rId3"/>
     <sheet name="4-Barricade" sheetId="4" r:id="rId4"/>
     <sheet name="5-Binding" sheetId="5" r:id="rId5"/>
-    <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
+    <sheet name="6-Gardna" sheetId="6" r:id="rId6"/>
     <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
     <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -225,13 +225,70 @@
   </si>
   <si>
     <t>I'll protect my allies the same way the gods protect me.</t>
+  </si>
+  <si>
+    <t>Gardna</t>
+  </si>
+  <si>
+    <t>[[Range: 1-2 ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: No ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell]]</t>
+  </si>
+  <si>
+    <t>Can't use the skill if there already a Gardna in the same team.</t>
+  </si>
+  <si>
+    <t>Can only be summoned on empty cell.</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 7 ]]</t>
+  </si>
+  <si>
+    <t>Gardna skill</t>
+  </si>
+  <si>
+    <t>Spirit Shield</t>
+  </si>
+  <si>
+    <t>Summon a ''Gardna'' [[1 HP, 3 AP, 1 MP, 1000% earth resistence, -1000% fire resistence, 1000% water resistence, 1000% air resistence, 1000% light resistence, 1000% dark resistence]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 1 ]]</t>
+  </si>
+  <si>
+    <t>Only affect self and allies</t>
+  </si>
+  <si>
+    <t>[[Boost HP by 20% of max HP of the affected target]] (2 turn)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Spirit Shield''.</t>
+  </si>
+  <si>
+    <t>[[Boost  resistance by 15%]] (1 turn)</t>
+  </si>
+  <si>
+    <t>A protective wave emanating from the spirit</t>
+  </si>
+  <si>
+    <t>To protect the gods will, divines spirits</t>
+  </si>
+  <si>
+    <t>allow me to summon them.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +320,16 @@
       <name val="Algerian"/>
       <family val="5"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,8 +354,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -307,11 +378,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -337,6 +432,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,7 +758,7 @@
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1138,7 @@
   <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,7 +1457,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1693,214 +1796,290 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
     <col min="7" max="7" width="78.5703125" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="1"/>
+      <c r="G1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F3" s="1"/>
+      <c r="G3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F4" s="1"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F5" s="1"/>
+      <c r="G5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F7" s="1"/>
+      <c r="G7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F9" s="1"/>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F10" s="1"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F11" s="1"/>
+      <c r="G11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F12" s="1"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F13" s="1"/>
+      <c r="G13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F15" s="1"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F17" s="1"/>
+      <c r="G17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="2:8" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F19" s="1"/>
+      <c r="G19" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="11"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F20" s="1"/>
+      <c r="G20" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F24" s="1"/>
+      <c r="G24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+      <c r="G26" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 1 skill in Guardian doc. (a big one)
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Guardian/Documentation/GuardianSkills.xlsx
+++ b/GameDesign/Class/Guardian/Documentation/GuardianSkills.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\Guardian\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1-ArmorStrengthening" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="4-Barricade" sheetId="4" r:id="rId4"/>
     <sheet name="5-Binding" sheetId="5" r:id="rId5"/>
     <sheet name="6-Gardna" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
-    <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
-    <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
-    <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
+    <sheet name="7-WillOfDestruction" sheetId="7" r:id="rId7"/>
+    <sheet name="8-SpiritFusion" sheetId="8" r:id="rId8"/>
+    <sheet name="9-MetallicTornado" sheetId="9" r:id="rId9"/>
+    <sheet name="10-DefensiveCharge" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -74,15 +74,6 @@
     <t>EX: [[Boost taken damage by 10%]] (2 turns)</t>
   </si>
   <si>
-    <t>SKILL DESCRIPTION</t>
-  </si>
-  <si>
-    <t>¨¨ ¨¨</t>
-  </si>
-  <si>
-    <t>SKILL NAME</t>
-  </si>
-  <si>
     <t>Effect name: ''X''.</t>
   </si>
   <si>
@@ -282,6 +273,84 @@
   </si>
   <si>
     <t>allow me to summon them.</t>
+  </si>
+  <si>
+    <t>Will Of Destruction</t>
+  </si>
+  <si>
+    <t>Alright I'm tired of their shit! They pushed their heresis too far!</t>
+  </si>
+  <si>
+    <t>I'LL KILL THEM ALL!</t>
+  </si>
+  <si>
+    <t>Effect name: ''Will Of Destruction''.</t>
+  </si>
+  <si>
+    <t>[[Will Of Destruction]] (2 turn)</t>
+  </si>
+  <si>
+    <t>[[Boost damage by 25%]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Reduct resistance by 25%]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 8 ]]</t>
+  </si>
+  <si>
+    <t>Prevent using those skills: [Armor Strengthening] - [Omniscient Shield] - [Backfire] - [Barricade] - [Gardna]</t>
+  </si>
+  <si>
+    <t>Transform this skill for ''Sword Of Destruction''</t>
+  </si>
+  <si>
+    <t>Can't be used if under ''Will Of Destruction'' effect.</t>
+  </si>
+  <si>
+    <t>Can't be used if the summoner under ''Will Of Destruction'' effect.</t>
+  </si>
+  <si>
+    <t>Unbuff all effects from self and Gardna on self and allies. (before giving this skill effects)</t>
+  </si>
+  <si>
+    <t>Metallic Tornado</t>
+  </si>
+  <si>
+    <t>Defensive Charge</t>
+  </si>
+  <si>
+    <t>Spirit Fusion</t>
+  </si>
+  <si>
+    <t>Change damage element of [Metallic Tornado] and [Defensive Charge] to Light.</t>
+  </si>
+  <si>
+    <t>2nd form skill</t>
+  </si>
+  <si>
+    <t>Sword Of Destruction</t>
+  </si>
+  <si>
+    <t>The sword of the god of destruction. Allow to destroy the</t>
+  </si>
+  <si>
+    <t>body and the soul of heretics with the permission of god.</t>
+  </si>
+  <si>
+    <t>[[MP: Remaning ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  [50 light + 50 earth] + [25 light * MP consumed] ]]</t>
+  </si>
+  <si>
+    <t>Only available if player under ''Will Of Destruction'' effect.</t>
+  </si>
+  <si>
+    <t>Turn back into ''Will Of Destruction'' skill when the player get out of ''Will Of Destruction'' effect.</t>
   </si>
 </sst>
 </file>
@@ -406,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -440,6 +509,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D25"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +874,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -790,7 +886,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -802,14 +898,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -821,7 +917,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -833,14 +929,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -852,7 +948,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -864,7 +960,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -894,21 +990,28 @@
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="6"/>
+      <c r="C25" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -921,7 +1024,7 @@
   <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +1044,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -952,16 +1055,12 @@
     </row>
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="9"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -1024,7 +1123,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1111,14 +1210,14 @@
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
       <c r="C31" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
       <c r="C32" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -1134,162 +1233,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D24"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B21" s="1"/>
-      <c r="C21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B23" s="1"/>
-      <c r="C23" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D25"/>
   <sheetViews>
@@ -1314,7 +1257,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1326,7 +1269,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1338,14 +1281,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1357,7 +1300,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1369,14 +1312,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1388,7 +1331,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1400,7 +1343,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1430,14 +1373,14 @@
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="10" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -1452,179 +1395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
@@ -1649,7 +1420,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1661,7 +1432,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1673,45 +1444,45 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>61</v>
+      <c r="C13" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1723,7 +1494,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1735,14 +1506,186 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>62</v>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B21" s="1"/>
+      <c r="C21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B23" s="1"/>
+      <c r="C23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D27"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1772,14 +1715,191 @@
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="10" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D26"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1796,10 +1916,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H28"/>
+  <dimension ref="B1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,7 +1936,7 @@
     <row r="1" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -1831,12 +1951,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1851,19 +1971,19 @@
     <row r="5" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1"/>
       <c r="F6" s="1"/>
@@ -1876,14 +1996,14 @@
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -1893,12 +2013,12 @@
     <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -1913,19 +2033,19 @@
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
@@ -1935,12 +2055,12 @@
     <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -1955,7 +2075,7 @@
     <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -1973,12 +2093,12 @@
     <row r="17" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1993,12 +2113,12 @@
     <row r="19" spans="2:8" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2008,7 +2128,7 @@
       <c r="D20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -2052,34 +2172,46 @@
     <row r="26" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="39" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="C28" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="14"/>
+      <c r="G28" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="6"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2089,10 +2221,351 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="1"/>
+      <c r="G1" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="1"/>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="1"/>
+      <c r="C28" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="1"/>
+      <c r="C30" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="1"/>
+      <c r="C31" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="2:8" ht="39" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,8 +2584,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
+      <c r="C3" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2123,16 +2596,12 @@
     </row>
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="9"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2195,7 +2664,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2282,14 +2751,14 @@
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
       <c r="C31" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
       <c r="C32" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -2304,12 +2773,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,7 +2798,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2340,16 +2809,12 @@
     </row>
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="9"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2412,7 +2877,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2499,231 +2964,14 @@
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
       <c r="C31" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
       <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added one skill in guardian doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Guardian/Documentation/GuardianSkills.xlsx
+++ b/GameDesign/Class/Guardian/Documentation/GuardianSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="1-ArmorStrengthening" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="113">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -257,9 +257,6 @@
     <t>Only affect self and allies</t>
   </si>
   <si>
-    <t>[[Boost HP by 20% of max HP of the affected target]] (2 turn)</t>
-  </si>
-  <si>
     <t>Effect name: ''Spirit Shield''.</t>
   </si>
   <si>
@@ -351,6 +348,30 @@
   </si>
   <si>
     <t>Turn back into ''Will Of Destruction'' skill when the player get out of ''Will Of Destruction'' effect.</t>
+  </si>
+  <si>
+    <t>[[Boost HP by 20% of max HP of the affected target]] (2 turns)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Spirit Fusion''.</t>
+  </si>
+  <si>
+    <t>if not under ''Will Of Destruction'' effect, Self: [[Boost resistance by 15%]] (2 turns)</t>
+  </si>
+  <si>
+    <t>if not under ''Will Of Destruction'' effect, Self: [[Boost HP by 20% of the guardian]] (2 turns)</t>
+  </si>
+  <si>
+    <t>Can only target the ''Gardna'' summon of this gardian.</t>
+  </si>
+  <si>
+    <t>Unsummon the ''Gardna''.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i'm not afraid to depends on spirit. They'll support me </t>
+  </si>
+  <si>
+    <t>no matter what to serve the gods higher interest.</t>
   </si>
 </sst>
 </file>
@@ -475,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -536,6 +557,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1004,7 +1028,7 @@
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1044,7 +1068,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1380,7 +1404,7 @@
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -1550,7 +1574,7 @@
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1729,7 +1753,7 @@
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -1971,19 +1995,19 @@
     <row r="5" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="1"/>
       <c r="F6" s="1"/>
@@ -2118,7 +2142,7 @@
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2128,7 +2152,7 @@
       <c r="D20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="15" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -2177,7 +2201,7 @@
       <c r="D26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H26" s="1"/>
     </row>
@@ -2196,12 +2220,12 @@
     <row r="28" spans="2:8" ht="39" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
       <c r="C28" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H28" s="13"/>
     </row>
@@ -2224,7 +2248,7 @@
   <dimension ref="B1:H33"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,7 +2265,7 @@
     <row r="1" spans="2:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2256,12 +2280,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2276,24 +2300,24 @@
     <row r="5" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -2323,7 +2347,7 @@
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -2335,7 +2359,7 @@
       <c r="D10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -2370,7 +2394,7 @@
     <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
@@ -2418,19 +2442,19 @@
     <row r="19" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="1"/>
       <c r="F20" s="1"/>
@@ -2440,7 +2464,7 @@
     <row r="21" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="1"/>
       <c r="F21" s="1"/>
@@ -2495,31 +2519,31 @@
     <row r="28" spans="2:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
       <c r="C28" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="2:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
       <c r="C29" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B30" s="1"/>
       <c r="C30" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="1"/>
       <c r="F30" s="1"/>
@@ -2529,7 +2553,7 @@
     <row r="31" spans="2:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B31" s="1"/>
       <c r="C31" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D31" s="1"/>
       <c r="F31" s="1"/>
@@ -2539,7 +2563,7 @@
     <row r="32" spans="2:8" ht="39" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
       <c r="C32" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D32" s="1"/>
       <c r="F32" s="1"/>
@@ -2561,6 +2585,209 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D31"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="1"/>
+      <c r="C21" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="1"/>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="1"/>
+      <c r="C28" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="1"/>
+      <c r="C30" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
@@ -2584,8 +2811,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="21" t="s">
-        <v>95</v>
+      <c r="C3" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2771,217 +2998,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B6" s="1"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>